<commit_message>
Added executive wise sales and so on
</commit_message>
<xml_diff>
--- a/Data/NoSales.xlsx
+++ b/Data/NoSales.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="65">
   <si>
     <t>BSL NO</t>
   </si>
@@ -31,79 +31,184 @@
     <t>UOM</t>
   </si>
   <si>
-    <t>Altadin</t>
-  </si>
-  <si>
-    <t>Betagan</t>
-  </si>
-  <si>
-    <t>Bimatol</t>
-  </si>
-  <si>
-    <t>Binzotim</t>
-  </si>
-  <si>
-    <t>Dextor OPT</t>
-  </si>
-  <si>
-    <t>Fluflam</t>
-  </si>
-  <si>
-    <t>Lotrel</t>
-  </si>
-  <si>
-    <t>Poly Pred</t>
-  </si>
-  <si>
-    <t>Pred OPT</t>
-  </si>
-  <si>
-    <t>Zolopt</t>
-  </si>
-  <si>
-    <t>Zymar</t>
-  </si>
-  <si>
-    <t>Altadin 0.25% Ophthalmic Solution</t>
-  </si>
-  <si>
-    <t>Betagan 0.5% 5 ml</t>
-  </si>
-  <si>
-    <t>Bimatol 5ml Ophthalmic Solution</t>
-  </si>
-  <si>
-    <t>Binzotim Ophthalmic Suspension 5ml</t>
-  </si>
-  <si>
-    <t>Dextor T Ophthalmic Suspension, 5ml</t>
-  </si>
-  <si>
-    <t>Fluflam 0.1% Opthalmic Suspension</t>
-  </si>
-  <si>
-    <t>Lotrel 0.5% Opthalmic Suspension</t>
-  </si>
-  <si>
-    <t>Poly Pred 5ml</t>
-  </si>
-  <si>
-    <t>PRED 5ml Ophthalmic Suspension</t>
-  </si>
-  <si>
-    <t>Zolopt Ophthalmic Suspension 5ml</t>
-  </si>
-  <si>
-    <t>Zymar 5ml</t>
-  </si>
-  <si>
-    <t>1's</t>
-  </si>
-  <si>
-    <t>5 ml.</t>
-  </si>
-  <si>
-    <t>5ml</t>
+    <t>Desodin</t>
+  </si>
+  <si>
+    <t>Dinafex</t>
+  </si>
+  <si>
+    <t>Dorenta</t>
+  </si>
+  <si>
+    <t>Etorix</t>
+  </si>
+  <si>
+    <t>Fenobac</t>
+  </si>
+  <si>
+    <t>Flucloxin</t>
+  </si>
+  <si>
+    <t>Geminox</t>
+  </si>
+  <si>
+    <t>Ketonic</t>
+  </si>
+  <si>
+    <t>Kynol</t>
+  </si>
+  <si>
+    <t>Naprox</t>
+  </si>
+  <si>
+    <t>Oradin</t>
+  </si>
+  <si>
+    <t>Osticare</t>
+  </si>
+  <si>
+    <t>Sk-Mox</t>
+  </si>
+  <si>
+    <t>Zithrox</t>
+  </si>
+  <si>
+    <t>Desodin 60ml Syrup</t>
+  </si>
+  <si>
+    <t>Dinafex 60mg Tablet</t>
+  </si>
+  <si>
+    <t>Dinafex 120mg Tablet</t>
+  </si>
+  <si>
+    <t>Dinafex 180mg Tablet</t>
+  </si>
+  <si>
+    <t>Dorenta 50mg Tablet</t>
+  </si>
+  <si>
+    <t>Etorix 60mg Tablet - 40's</t>
+  </si>
+  <si>
+    <t>Etorix 120mg Tablet</t>
+  </si>
+  <si>
+    <t>Etorix 90mg Tablet</t>
+  </si>
+  <si>
+    <t>Fenobac 100ml Syrup</t>
+  </si>
+  <si>
+    <t>Flucloxin 500mg Capsule - 36's</t>
+  </si>
+  <si>
+    <t>Flucloxin 500mg Capsule</t>
+  </si>
+  <si>
+    <t>Geminox 320mg Tablet - 8's</t>
+  </si>
+  <si>
+    <t>Ketonic 30mg Injection</t>
+  </si>
+  <si>
+    <t>Ketonic 30mg IM/IV Injection - 4's</t>
+  </si>
+  <si>
+    <t>Ketonic 10mg Tablet</t>
+  </si>
+  <si>
+    <t>Kynol TR 100mg Capsule</t>
+  </si>
+  <si>
+    <t>Kynol D 25mg Tablet</t>
+  </si>
+  <si>
+    <t>Kynol TR 200mg Capsule</t>
+  </si>
+  <si>
+    <t>Naprox Plus 500mg Tablet - 30's</t>
+  </si>
+  <si>
+    <t>Oradin Plus Tablet - 40's</t>
+  </si>
+  <si>
+    <t>Osticare Tablet 24's</t>
+  </si>
+  <si>
+    <t>Sk-Mox 500mg Capsule</t>
+  </si>
+  <si>
+    <t>Zithrox 250mg Tablet - 6's</t>
+  </si>
+  <si>
+    <t>Zithrox 15ml Suspension</t>
+  </si>
+  <si>
+    <t>Zithrox 500mg Tablet</t>
+  </si>
+  <si>
+    <t>Zithrox 30ml Dry Suspension</t>
+  </si>
+  <si>
+    <t>60 ml</t>
+  </si>
+  <si>
+    <t>30's</t>
+  </si>
+  <si>
+    <t>50's</t>
+  </si>
+  <si>
+    <t>40's</t>
+  </si>
+  <si>
+    <t>20's</t>
+  </si>
+  <si>
+    <t>100ml</t>
+  </si>
+  <si>
+    <t>36 's</t>
+  </si>
+  <si>
+    <t>30 's</t>
+  </si>
+  <si>
+    <t>8 's</t>
+  </si>
+  <si>
+    <t>5 's</t>
+  </si>
+  <si>
+    <t>4's</t>
+  </si>
+  <si>
+    <t>50 's</t>
+  </si>
+  <si>
+    <t>60 's</t>
+  </si>
+  <si>
+    <t>40 's</t>
+  </si>
+  <si>
+    <t>24's</t>
+  </si>
+  <si>
+    <t>48 's</t>
+  </si>
+  <si>
+    <t>6's</t>
+  </si>
+  <si>
+    <t>15 ml</t>
+  </si>
+  <si>
+    <t>6 's</t>
+  </si>
+  <si>
+    <t>30ml</t>
   </si>
 </sst>
 </file>
@@ -461,7 +566,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -486,7 +591,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -495,15 +600,15 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -512,10 +617,10 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -523,152 +628,407 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
         <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C10">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E11" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C12">
         <v>11</v>
       </c>
       <c r="D12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15">
+        <v>14</v>
+      </c>
+      <c r="D15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16">
+        <v>15</v>
+      </c>
+      <c r="D16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17">
+        <v>16</v>
+      </c>
+      <c r="D17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18">
+        <v>17</v>
+      </c>
+      <c r="D18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>12</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19">
+        <v>18</v>
+      </c>
+      <c r="D19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20">
+        <v>19</v>
+      </c>
+      <c r="D20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21">
+        <v>20</v>
+      </c>
+      <c r="D21" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22">
+        <v>21</v>
+      </c>
+      <c r="D22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23">
+        <v>22</v>
+      </c>
+      <c r="D23" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24">
+        <v>35</v>
+      </c>
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24">
+        <v>23</v>
+      </c>
+      <c r="D24" t="s">
+        <v>41</v>
+      </c>
+      <c r="E24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25">
+        <v>35</v>
+      </c>
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25">
+        <v>24</v>
+      </c>
+      <c r="D25" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26">
+        <v>35</v>
+      </c>
+      <c r="B26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26">
+        <v>25</v>
+      </c>
+      <c r="D26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27">
+        <v>35</v>
+      </c>
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27">
         <v>26</v>
       </c>
-      <c r="E12" t="s">
-        <v>29</v>
+      <c r="D27" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add branch wise stocks
</commit_message>
<xml_diff>
--- a/Data/NoSales.xlsx
+++ b/Data/NoSales.xlsx
@@ -76,57 +76,57 @@
     <t>Desodin 60ml Syrup</t>
   </si>
   <si>
+    <t>Dinafex 180mg Tablet</t>
+  </si>
+  <si>
     <t>Dinafex 120mg Tablet</t>
   </si>
   <si>
     <t>Dinafex 60mg Tablet</t>
   </si>
   <si>
-    <t>Dinafex 180mg Tablet</t>
-  </si>
-  <si>
     <t>Dorenta 50mg Tablet</t>
   </si>
   <si>
+    <t>Etorix 120mg Tablet</t>
+  </si>
+  <si>
     <t>Etorix 60mg Tablet - 40's</t>
   </si>
   <si>
     <t>Etorix 90mg Tablet</t>
   </si>
   <si>
-    <t>Etorix 120mg Tablet</t>
-  </si>
-  <si>
     <t>Fenobac 100ml Syrup</t>
   </si>
   <si>
+    <t>Flucloxin 500mg Capsule</t>
+  </si>
+  <si>
     <t>Flucloxin 500mg Capsule - 36's</t>
   </si>
   <si>
-    <t>Flucloxin 500mg Capsule</t>
-  </si>
-  <si>
     <t>Geminox 320mg Tablet - 8's</t>
   </si>
   <si>
     <t>Ketonic 30mg Injection</t>
   </si>
   <si>
+    <t>Ketonic 30mg IM/IV Injection - 4's</t>
+  </si>
+  <si>
     <t>Ketonic 10mg Tablet</t>
   </si>
   <si>
-    <t>Ketonic 30mg IM/IV Injection - 4's</t>
+    <t>Kynol D 25mg Tablet</t>
+  </si>
+  <si>
+    <t>Kynol TR 100mg Capsule</t>
   </si>
   <si>
     <t>Kynol TR 200mg Capsule</t>
   </si>
   <si>
-    <t>Kynol TR 100mg Capsule</t>
-  </si>
-  <si>
-    <t>Kynol D 25mg Tablet</t>
-  </si>
-  <si>
     <t>Naprox Plus 500mg Tablet - 30's</t>
   </si>
   <si>
@@ -139,18 +139,18 @@
     <t>Sk-Mox 500mg Capsule</t>
   </si>
   <si>
+    <t>Zithrox 30ml Dry Suspension</t>
+  </si>
+  <si>
     <t>Zithrox 15ml Suspension</t>
   </si>
   <si>
+    <t>Zithrox 250mg Tablet - 6's</t>
+  </si>
+  <si>
     <t>Zithrox 500mg Tablet</t>
   </si>
   <si>
-    <t>Zithrox 250mg Tablet - 6's</t>
-  </si>
-  <si>
-    <t>Zithrox 30ml Dry Suspension</t>
-  </si>
-  <si>
     <t>60 ml</t>
   </si>
   <si>
@@ -160,21 +160,21 @@
     <t>50's</t>
   </si>
   <si>
+    <t>20's</t>
+  </si>
+  <si>
     <t>40's</t>
   </si>
   <si>
-    <t>20's</t>
-  </si>
-  <si>
     <t>100ml</t>
   </si>
   <si>
+    <t>30 's</t>
+  </si>
+  <si>
     <t>36 's</t>
   </si>
   <si>
-    <t>30 's</t>
-  </si>
-  <si>
     <t>8 's</t>
   </si>
   <si>
@@ -184,12 +184,12 @@
     <t>4's</t>
   </si>
   <si>
+    <t>60 's</t>
+  </si>
+  <si>
     <t>50 's</t>
   </si>
   <si>
-    <t>60 's</t>
-  </si>
-  <si>
     <t>40 's</t>
   </si>
   <si>
@@ -199,16 +199,16 @@
     <t>48 's</t>
   </si>
   <si>
+    <t>30ml</t>
+  </si>
+  <si>
     <t>15 ml</t>
   </si>
   <si>
+    <t>6's</t>
+  </si>
+  <si>
     <t>6 's</t>
-  </si>
-  <si>
-    <t>6's</t>
-  </si>
-  <si>
-    <t>30ml</t>
   </si>
 </sst>
 </file>
@@ -705,7 +705,7 @@
         <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -722,7 +722,7 @@
         <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -824,7 +824,7 @@
         <v>32</v>
       </c>
       <c r="E15" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -841,7 +841,7 @@
         <v>33</v>
       </c>
       <c r="E16" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -858,7 +858,7 @@
         <v>34</v>
       </c>
       <c r="E17" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -875,7 +875,7 @@
         <v>35</v>
       </c>
       <c r="E18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -892,7 +892,7 @@
         <v>36</v>
       </c>
       <c r="E19" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -909,7 +909,7 @@
         <v>37</v>
       </c>
       <c r="E20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:5">

</xml_diff>

<commit_message>
branch wise stock status added
</commit_message>
<xml_diff>
--- a/Data/NoSales.xlsx
+++ b/Data/NoSales.xlsx
@@ -79,12 +79,12 @@
     <t>Dinafex 180mg Tablet</t>
   </si>
   <si>
+    <t>Dinafex 60mg Tablet</t>
+  </si>
+  <si>
     <t>Dinafex 120mg Tablet</t>
   </si>
   <si>
-    <t>Dinafex 60mg Tablet</t>
-  </si>
-  <si>
     <t>Dorenta 50mg Tablet</t>
   </si>
   <si>
@@ -109,24 +109,24 @@
     <t>Geminox 320mg Tablet - 8's</t>
   </si>
   <si>
+    <t>Ketonic 10mg Tablet</t>
+  </si>
+  <si>
+    <t>Ketonic 30mg IM/IV Injection - 4's</t>
+  </si>
+  <si>
     <t>Ketonic 30mg Injection</t>
   </si>
   <si>
-    <t>Ketonic 30mg IM/IV Injection - 4's</t>
-  </si>
-  <si>
-    <t>Ketonic 10mg Tablet</t>
+    <t>Kynol TR 100mg Capsule</t>
+  </si>
+  <si>
+    <t>Kynol TR 200mg Capsule</t>
   </si>
   <si>
     <t>Kynol D 25mg Tablet</t>
   </si>
   <si>
-    <t>Kynol TR 100mg Capsule</t>
-  </si>
-  <si>
-    <t>Kynol TR 200mg Capsule</t>
-  </si>
-  <si>
     <t>Naprox Plus 500mg Tablet - 30's</t>
   </si>
   <si>
@@ -139,18 +139,18 @@
     <t>Sk-Mox 500mg Capsule</t>
   </si>
   <si>
+    <t>Zithrox 15ml Suspension</t>
+  </si>
+  <si>
+    <t>Zithrox 250mg Tablet - 6's</t>
+  </si>
+  <si>
+    <t>Zithrox 500mg Tablet</t>
+  </si>
+  <si>
     <t>Zithrox 30ml Dry Suspension</t>
   </si>
   <si>
-    <t>Zithrox 15ml Suspension</t>
-  </si>
-  <si>
-    <t>Zithrox 250mg Tablet - 6's</t>
-  </si>
-  <si>
-    <t>Zithrox 500mg Tablet</t>
-  </si>
-  <si>
     <t>60 ml</t>
   </si>
   <si>
@@ -178,18 +178,18 @@
     <t>8 's</t>
   </si>
   <si>
+    <t>4's</t>
+  </si>
+  <si>
     <t>5 's</t>
   </si>
   <si>
-    <t>4's</t>
+    <t>50 's</t>
   </si>
   <si>
     <t>60 's</t>
   </si>
   <si>
-    <t>50 's</t>
-  </si>
-  <si>
     <t>40 's</t>
   </si>
   <si>
@@ -199,16 +199,16 @@
     <t>48 's</t>
   </si>
   <si>
+    <t>15 ml</t>
+  </si>
+  <si>
+    <t>6's</t>
+  </si>
+  <si>
+    <t>6 's</t>
+  </si>
+  <si>
     <t>30ml</t>
-  </si>
-  <si>
-    <t>15 ml</t>
-  </si>
-  <si>
-    <t>6's</t>
-  </si>
-  <si>
-    <t>6 's</t>
   </si>
 </sst>
 </file>
@@ -807,7 +807,7 @@
         <v>31</v>
       </c>
       <c r="E14" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -824,7 +824,7 @@
         <v>32</v>
       </c>
       <c r="E15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -841,7 +841,7 @@
         <v>33</v>
       </c>
       <c r="E16" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -875,7 +875,7 @@
         <v>35</v>
       </c>
       <c r="E18" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -892,7 +892,7 @@
         <v>36</v>
       </c>
       <c r="E19" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:5">

</xml_diff>